<commit_message>
updation in register feature
</commit_message>
<xml_diff>
--- a/TestData/login_data.xlsx
+++ b/TestData/login_data.xlsx
@@ -5,16 +5,23 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PilotProject_Cyclos_Team1\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PilotProject_Cyclos_Team1-1\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E3B274A-C432-43DC-B3B7-8EB5FE4676E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73815934-128E-44DD-A174-D88C47AB7E11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="invalidLogin" sheetId="1" r:id="rId1"/>
-    <sheet name="validLogin" sheetId="2" r:id="rId2"/>
+    <sheet name="validRegister" sheetId="3" r:id="rId2"/>
+    <sheet name="invalidPassword" sheetId="4" r:id="rId3"/>
+    <sheet name="confirmPassword" sheetId="5" r:id="rId4"/>
+    <sheet name="validatingBlank" sheetId="6" r:id="rId5"/>
+    <sheet name="mandatoryField" sheetId="7" r:id="rId6"/>
+    <sheet name="invalidEmail" sheetId="8" r:id="rId7"/>
+    <sheet name="alreadyEmail" sheetId="9" r:id="rId8"/>
+    <sheet name="validLogin" sheetId="2" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="39">
   <si>
     <t>Sand@123</t>
   </si>
@@ -62,6 +69,87 @@
   </si>
   <si>
     <t>Sahana123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  abc</t>
+  </si>
+  <si>
+    <t>${login}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${email} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">${website} </t>
+  </si>
+  <si>
+    <t>abc12345</t>
+  </si>
+  <si>
+    <t>www.google.com</t>
+  </si>
+  <si>
+    <t>${name}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${gender} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">${mobile} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">${land_line} </t>
+  </si>
+  <si>
+    <t>${address}</t>
+  </si>
+  <si>
+    <t>${zip}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${city} </t>
+  </si>
+  <si>
+    <t>${region}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${password} </t>
+  </si>
+  <si>
+    <t>${confirm_password}</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>(201) 555-0123</t>
+  </si>
+  <si>
+    <t>gandhi street</t>
+  </si>
+  <si>
+    <t>salem</t>
+  </si>
+  <si>
+    <t>tamilnadu</t>
+  </si>
+  <si>
+    <t>abc@123</t>
+  </si>
+  <si>
+    <t>abc123@gmail.com</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>abc@124</t>
+  </si>
+  <si>
+    <t>abc123@gmail.</t>
+  </si>
+  <si>
+    <t>sandhiya110902@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -106,9 +194,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -392,7 +483,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
@@ -437,6 +528,573 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF64E1AF-B64A-4B3C-BD19-9A98FDB28A22}">
+  <dimension ref="A1:M11"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="24.77734375" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5546875" customWidth="1"/>
+    <col min="8" max="8" width="13.5546875" customWidth="1"/>
+    <col min="12" max="12" width="12.44140625" customWidth="1"/>
+    <col min="13" max="13" width="21.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2">
+        <v>9856743210</v>
+      </c>
+      <c r="G2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2">
+        <v>637503</v>
+      </c>
+      <c r="J2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B11" s="2"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{D2D43A7C-8E90-4F49-8E75-398C17D4BF47}"/>
+    <hyperlink ref="L2" r:id="rId2" xr:uid="{B94A7252-DFE6-4BB4-A9C8-1F99B19664E7}"/>
+    <hyperlink ref="M2" r:id="rId3" xr:uid="{76C8326E-C84B-4A3E-9B53-680B6B93DF73}"/>
+    <hyperlink ref="C2" r:id="rId4" xr:uid="{5EDE5545-EFBB-424D-A276-501A562F7F69}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62AAE4BB-23F8-4DC4-8253-050E3A8F1738}">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.77734375" customWidth="1"/>
+    <col min="4" max="4" width="10.77734375" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" customWidth="1"/>
+    <col min="9" max="9" width="10.21875" customWidth="1"/>
+    <col min="10" max="10" width="11" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" customWidth="1"/>
+    <col min="12" max="12" width="18.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2">
+        <v>9856743210</v>
+      </c>
+      <c r="F2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2">
+        <v>637503</v>
+      </c>
+      <c r="I2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{190E00DA-A976-45E7-93D6-79B0F5A724D6}"/>
+    <hyperlink ref="K2" r:id="rId2" display="abc@123" xr:uid="{9F94E111-56E2-460B-B0F7-C97B13C7806C}"/>
+    <hyperlink ref="L2" r:id="rId3" xr:uid="{BBF0D27C-0171-4849-8FF9-C46E8B589EF7}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{4294A91F-2202-487D-ACB2-FA5BB6245A90}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{897AAAF8-CD28-4887-B39B-6EAAFBAB94BD}">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="19.77734375" customWidth="1"/>
+    <col min="4" max="4" width="16.44140625" customWidth="1"/>
+    <col min="6" max="7" width="15.5546875" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
+    <col min="12" max="12" width="13.109375" customWidth="1"/>
+    <col min="13" max="13" width="19.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2">
+        <v>9856743210</v>
+      </c>
+      <c r="G2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2">
+        <v>637503</v>
+      </c>
+      <c r="J2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{9F07DB1D-55F0-4BAD-AB4A-EE29002173BB}"/>
+    <hyperlink ref="L2" r:id="rId2" xr:uid="{426E22AF-B0C1-4942-8A1D-2D244F0DBB2F}"/>
+    <hyperlink ref="M2" r:id="rId3" xr:uid="{F44D058D-49F3-4EFF-ACB0-358F30C21AD5}"/>
+    <hyperlink ref="C2" r:id="rId4" xr:uid="{710CA2C7-730B-48EF-8A0C-6F1FA1200894}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BFDBF8C-E990-465C-AEA0-C79208D80B48}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.88671875" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" customWidth="1"/>
+    <col min="4" max="4" width="16.77734375" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.21875" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2">
+        <v>9856743210</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2">
+        <v>637503</v>
+      </c>
+      <c r="G2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{93C035F3-5684-4991-9930-787D0B8F488D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E594A082-7D03-46B7-AFEC-B5F0370087A6}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10.77734375" customWidth="1"/>
+    <col min="5" max="5" width="19.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{D244684C-E539-461A-949D-305C2D258968}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{505BC845-F39A-463D-9FFF-9E3800626574}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{792EC99E-7284-4209-A598-185353D4698D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A8DBF35-695C-44A3-AD3A-3B205B2CA974}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="17.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{800CD8A4-B317-4197-8B43-D2A65DDF77C8}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32B9F295-44F1-4B6E-860F-99E1A9E7D4B5}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="25.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{2A463C6B-2388-46F2-BC9A-AC88D9AA5D6C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC1D071C-D4BB-4BA4-8801-973517A97F3B}">
   <dimension ref="A1:B4"/>
   <sheetViews>

</xml_diff>